<commit_message>
Arreglos varios + New songs
</commit_message>
<xml_diff>
--- a/BasketLeague/Data/FrikiLeague.xlsx
+++ b/BasketLeague/Data/FrikiLeague.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IanLiceranzu\source\repos\BasketLeague\BasketLeague\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71168870-8CC1-4ABB-9876-2ED1B3B155E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4507DFC7-25BC-4B6D-8FAF-62D87B5FA7EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>N</t>
   </si>
@@ -63,52 +63,37 @@
     <t>RESULTADO</t>
   </si>
   <si>
-    <t>Seattle Killer Whales</t>
+    <t>Boston Frogfish</t>
   </si>
   <si>
-    <t>PLAYOFFS</t>
+    <t>Columbus Tequila Splitfish</t>
   </si>
   <si>
-    <t>MP</t>
+    <t>Dallas Tiger Sharks</t>
   </si>
   <si>
-    <t>JP</t>
+    <t>Pukalami Clownfish</t>
   </si>
   <si>
-    <t>Boston Frogs</t>
+    <t>Jackson Huso Husos</t>
   </si>
   <si>
-    <t>THB</t>
+    <t>Kansas Blowfish</t>
   </si>
   <si>
-    <t>BF</t>
+    <t>Baltimore Barracudas</t>
   </si>
   <si>
-    <t>Milwaukee Platypus</t>
+    <t>Waukesha Panfish</t>
   </si>
   <si>
-    <t>Reno Bighorns</t>
+    <t>Sun Valley Sunfish</t>
   </si>
   <si>
-    <t>Tampa Honey Bagers</t>
+    <t>Walla Walla Mullets</t>
   </si>
   <si>
-    <t>Dallas Squirrels</t>
-  </si>
-  <si>
-    <t>Jackson Pandas</t>
-  </si>
-  <si>
-    <t>Kansas Kangaroos</t>
-  </si>
-  <si>
-    <t>Little Rock Wombats</t>
-  </si>
-  <si>
-    <t>Honolulu Meerkats</t>
-  </si>
-  <si>
-    <t>Columbus Hellbenders</t>
+    <t>Pensacola Kois</t>
   </si>
 </sst>
 </file>
@@ -140,18 +125,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -275,8 +254,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,7 +457,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4597E025-3453-4060-B6C7-90717D6EED2F}" name="Tabla1" displayName="Tabla1" ref="A1:G12" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:G12" xr:uid="{3959D846-4D1F-4F18-8DD2-42832383763C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-    <sortCondition descending="1" ref="D1:D12"/>
+    <sortCondition ref="B1:B12"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{68B6D7FA-C431-4729-B763-F126577D8D4B}" name="N" dataDxfId="6"/>
@@ -759,13 +738,13 @@
   <dimension ref="A1:AD72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
@@ -816,7 +795,7 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -836,25 +815,13 @@
       <c r="G2" s="8">
         <v>0</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="H2" s="17"/>
       <c r="M2" s="15"/>
-      <c r="N2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="11">
-        <v>103</v>
-      </c>
-      <c r="Q2" s="11">
-        <v>111</v>
-      </c>
-      <c r="R2" s="11">
-        <v>-8</v>
-      </c>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="15"/>
       <c r="U2" s="15"/>
@@ -870,43 +837,33 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="7">
         <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="H3" s="17"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="11">
-        <v>120</v>
-      </c>
-      <c r="Q3" s="11">
-        <v>106</v>
-      </c>
-      <c r="R3" s="11">
-        <v>14</v>
-      </c>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
@@ -922,25 +879,25 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7">
         <v>0</v>
       </c>
       <c r="G4" s="6">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="H4" s="17"/>
       <c r="M4" s="12"/>
@@ -964,10 +921,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -1006,25 +963,25 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
       </c>
       <c r="F6" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="6">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="11"/>
@@ -1047,10 +1004,10 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -1088,25 +1045,25 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
       </c>
       <c r="F8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="11"/>
@@ -1129,10 +1086,10 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -1170,10 +1127,10 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -1211,10 +1168,10 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -1252,10 +1209,10 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
@@ -1266,7 +1223,9 @@
       <c r="E12" s="9">
         <v>0</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
       <c r="G12" s="9">
         <v>0</v>
       </c>
@@ -2490,9 +2449,8 @@
       <c r="AD72" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="H2:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>